<commit_message>
Create script for comparing workbooks, WIP
</commit_message>
<xml_diff>
--- a/TestCases/CreateSheetsFromTemplate/TalismanTestData.xlsx
+++ b/TestCases/CreateSheetsFromTemplate/TalismanTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD040F7-5BCA-4C79-9166-DCCD0D788726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442E25F3-9E8E-4B71-99D8-2C070FBFCBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="2985" windowWidth="21600" windowHeight="11385" firstSheet="29" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2715" yWindow="2985" windowWidth="21600" windowHeight="11385" firstSheet="32" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="26" r:id="rId1"/>
@@ -48,6 +48,8 @@
     <sheet name="Dylan" sheetId="38" r:id="rId38"/>
     <sheet name="Fionn" sheetId="39" r:id="rId39"/>
     <sheet name="Felix" sheetId="40" r:id="rId40"/>
+    <sheet name="Names (13)" sheetId="41" r:id="rId41"/>
+    <sheet name="Names (14)" sheetId="42" r:id="rId42"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="34">
   <si>
     <t>Email</t>
   </si>
@@ -3686,10 +3688,164 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF887CF-EA7A-44B1-9DB7-DF1A35DD4624}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA566ED1-B290-417D-AEB7-D52CCAD09E0E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C778F238-8DF4-4D1D-A554-7B1E9ED2D3D7}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="20">
+        <v>3</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <f>AVERAGE(A8:D8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F849490D-C918-4DBD-93C3-7B10C1D6EFC7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>